<commit_message>
sim ve lgs hesaplama formülü eklendi
</commit_message>
<xml_diff>
--- a/Çınar.xlsx
+++ b/Çınar.xlsx
@@ -1,28 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5319165-7AE8-42F1-910E-8B2CEF8FD83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30F3EC-EF80-4E5E-8C01-40B315DBD8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Haftalık Plan" sheetId="1" r:id="rId1"/>
     <sheet name="Soru Çözüm Tablosu" sheetId="2" r:id="rId2"/>
     <sheet name="Okul Deneme Sonuç" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="71">
   <si>
     <t>Saat</t>
   </si>
@@ -228,13 +237,29 @@
   </si>
   <si>
     <t>GENEL TOPLAM</t>
+  </si>
+  <si>
+    <t>Puan</t>
+  </si>
+  <si>
+    <t>Net</t>
+  </si>
+  <si>
+    <t>Ağırlık</t>
+  </si>
+  <si>
+    <t>SİM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,8 +324,15 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +380,20 @@
         <fgColor rgb="FFA5A5A5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -406,32 +450,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -470,9 +488,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -501,86 +519,93 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="7" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="6" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="5" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="5" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -874,7 +899,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -995,10 +1020,10 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="30" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1011,8 +1036,8 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1023,10 +1048,10 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1039,8 +1064,8 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1051,10 +1076,10 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="30" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1067,8 +1092,8 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="14"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1079,10 +1104,10 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="14"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1093,8 +1118,8 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="17" t="s">
+      <c r="G13" s="25"/>
+      <c r="H13" s="23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1107,8 +1132,8 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="18"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1119,8 +1144,8 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="15" t="s">
+      <c r="G15" s="25"/>
+      <c r="H15" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1133,8 +1158,8 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="15"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="22"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -1155,8 +1180,8 @@
       <c r="F17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="22"/>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="30" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1164,34 +1189,34 @@
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="14"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="30"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="22"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="6" t="s">
         <v>15</v>
       </c>
@@ -1200,21 +1225,21 @@
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="14" t="s">
+      <c r="E20" s="22"/>
+      <c r="F20" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="22"/>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="25"/>
+      <c r="H20" s="30" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1222,39 +1247,39 @@
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="17" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="23" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="14"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="21" t="s">
+      <c r="D22" s="23"/>
+      <c r="E22" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="23" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1262,35 +1287,35 @@
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="19" t="s">
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="14" t="s">
+      <c r="D24" s="28"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="30" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1298,15 +1323,15 @@
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="15" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="22"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -1318,35 +1343,35 @@
       <c r="C26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="15"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="30" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="16" t="s">
+      <c r="G27" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="29" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1354,15 +1379,15 @@
       <c r="A28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="12" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
@@ -1380,8 +1405,8 @@
       <c r="E29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
       <c r="H29" s="2" t="s">
         <v>60</v>
       </c>
@@ -1390,8 +1415,8 @@
       <c r="A30" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
@@ -1406,17 +1431,17 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G12:G21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G22:G23"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="B20:B21"/>
@@ -1433,32 +1458,40 @@
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="D21:D22"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G12:G21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="H20:H21"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G8:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="69" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddHeader>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddFooter>
+    <evenHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenHeader>
+    <evenFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenFooter>
+    <firstHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstHeader>
+    <firstFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
+    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
@@ -1471,801 +1504,1191 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="30">
+      <c r="A2" s="32">
         <v>45549</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="33"/>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="35"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="35"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="35"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="35"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="32">
         <v>45550</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="32"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="35"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="35"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="32"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="35"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="32">
         <v>45551</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="32"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="35"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="35"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="35"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="35"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="32"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="35"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="32">
         <v>45552</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="32"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="33"/>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="35"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="35"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="34"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="30">
+      <c r="A30" s="32">
         <v>45553</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="32"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="35"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="32"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="35"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="32"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="35"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="32"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="33"/>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="32"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="35"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="32"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="35"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
-      <c r="G36" s="35"/>
-      <c r="H36" s="36"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="30">
+      <c r="A37" s="32">
         <v>45554</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="32"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="35"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="33"/>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="32"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="35"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="33"/>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="32"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="35"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="33"/>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="32"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="35"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="33"/>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="32"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="35"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="33"/>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="31"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="31"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="32"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="35"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="36"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="19"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="30">
+      <c r="A44" s="32">
         <v>45555</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="31"/>
-      <c r="H44" s="32"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="35"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="33"/>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="31"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="32"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="35"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="33"/>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="32"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="35"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="33"/>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="32"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="35"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="33"/>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="32"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="35"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="33"/>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="32"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="35"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="34" t="s">
         <v>59</v>
       </c>
       <c r="B50" s="34"/>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="35"/>
-      <c r="H50" s="36"/>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="37" t="s">
+      <c r="A51" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="39"/>
+      <c r="B51" s="31"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="H16:H21"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="H30:H35"/>
+    <mergeCell ref="H37:H42"/>
+    <mergeCell ref="H44:H49"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A37:A42"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:A49"/>
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A16:A21"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="H37:H42"/>
-    <mergeCell ref="H44:H49"/>
-    <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A37:A42"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="H16:H21"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="H30:H35"/>
     <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A44:A49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="97" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddHeader>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddFooter>
+    <evenHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenHeader>
+    <evenFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenFooter>
+    <firstHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstHeader>
+    <firstFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F8"/>
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
+  </sheetPr>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" style="1"/>
+    <col min="4" max="8" width="9.140625" style="1"/>
+    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+      <c r="G1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" s="41">
+        <v>194.752082</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="U1" s="41">
+        <v>194.752082</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="32">
         <v>45546</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="16">
         <v>20</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="16">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="16">
         <v>6</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" t="s">
+      <c r="G2" s="37">
+        <f>$D2-(E2/3)</f>
+        <v>8</v>
+      </c>
+      <c r="H2" s="39">
+        <v>4.2538</v>
+      </c>
+      <c r="I2" s="39">
+        <f>$G2*H2</f>
+        <v>34.0304</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="36">
+        <v>20</v>
+      </c>
+      <c r="O2" s="36">
+        <v>20</v>
+      </c>
+      <c r="P2" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="36">
+        <v>0</v>
+      </c>
+      <c r="R2" s="36">
+        <f>$O2-(P2/3)</f>
+        <v>20</v>
+      </c>
+      <c r="S2" s="36">
+        <v>4.2538</v>
+      </c>
+      <c r="T2" s="36">
+        <f>$R2*S2</f>
+        <v>85.075999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="16">
         <v>20</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="16">
         <v>14</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="16">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" t="s">
+      <c r="F3" s="16">
+        <v>0</v>
+      </c>
+      <c r="G3" s="37">
+        <f t="shared" ref="G3:G7" si="0">$D3-(E3/3)</f>
+        <v>12</v>
+      </c>
+      <c r="H3" s="39">
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="I3" s="39">
+        <f t="shared" ref="I3:I7" si="1">$G3*H3</f>
+        <v>52.176000000000002</v>
+      </c>
+      <c r="L3" s="33"/>
+      <c r="M3" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="N3" s="36">
+        <v>20</v>
+      </c>
+      <c r="O3" s="36">
+        <v>20</v>
+      </c>
+      <c r="P3" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="36">
+        <v>0</v>
+      </c>
+      <c r="R3" s="36">
+        <f t="shared" ref="R3:R7" si="2">$O3-(P3/3)</f>
+        <v>20</v>
+      </c>
+      <c r="S3" s="36">
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="T3" s="36">
+        <f t="shared" ref="T3:T7" si="3">$R3*S3</f>
+        <v>86.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="16">
         <v>20</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="16">
         <v>16</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="16">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
-      <c r="B5" t="s">
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="37">
+        <f t="shared" si="0"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="H4" s="39">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="I4" s="39">
+        <f t="shared" si="1"/>
+        <v>60.470666666666666</v>
+      </c>
+      <c r="L4" s="33"/>
+      <c r="M4" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="36">
+        <v>20</v>
+      </c>
+      <c r="O4" s="36">
+        <v>20</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="36">
+        <v>0</v>
+      </c>
+      <c r="R4" s="36">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="S4" s="36">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="T4" s="36">
+        <f t="shared" si="3"/>
+        <v>82.460000000000008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="15" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" t="s">
+      <c r="C5" s="36">
+        <v>10</v>
+      </c>
+      <c r="D5" s="36">
+        <v>10</v>
+      </c>
+      <c r="E5" s="36">
+        <v>0</v>
+      </c>
+      <c r="F5" s="36">
+        <v>0</v>
+      </c>
+      <c r="G5" s="38">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H5" s="40">
+        <v>1.66</v>
+      </c>
+      <c r="I5" s="40">
+        <f t="shared" si="1"/>
+        <v>16.599999999999998</v>
+      </c>
+      <c r="L5" s="33"/>
+      <c r="M5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="N5" s="36">
+        <v>10</v>
+      </c>
+      <c r="O5" s="36">
+        <v>10</v>
+      </c>
+      <c r="P5" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="36">
+        <v>0</v>
+      </c>
+      <c r="R5" s="36">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="S5" s="40">
+        <v>1.66</v>
+      </c>
+      <c r="T5" s="36">
+        <f t="shared" si="3"/>
+        <v>16.599999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" t="s">
+      <c r="C6" s="36">
+        <v>10</v>
+      </c>
+      <c r="D6" s="36">
+        <v>10</v>
+      </c>
+      <c r="E6" s="36">
+        <v>0</v>
+      </c>
+      <c r="F6" s="36">
+        <v>0</v>
+      </c>
+      <c r="G6" s="38">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H6" s="40">
+        <v>1.5075000000000001</v>
+      </c>
+      <c r="I6" s="40">
+        <f t="shared" si="1"/>
+        <v>15.075000000000001</v>
+      </c>
+      <c r="L6" s="33"/>
+      <c r="M6" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="36">
+        <v>10</v>
+      </c>
+      <c r="O6" s="36">
+        <v>10</v>
+      </c>
+      <c r="P6" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="36">
+        <v>0</v>
+      </c>
+      <c r="R6" s="36">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="S6" s="40">
+        <v>1.5075000000000001</v>
+      </c>
+      <c r="T6" s="36">
+        <f t="shared" si="3"/>
+        <v>15.075000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="C7" s="36">
+        <v>10</v>
+      </c>
+      <c r="D7" s="36">
+        <v>10</v>
+      </c>
+      <c r="E7" s="36">
+        <v>0</v>
+      </c>
+      <c r="F7" s="36">
+        <v>0</v>
+      </c>
+      <c r="G7" s="38">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H7" s="40">
+        <v>1.899</v>
+      </c>
+      <c r="I7" s="40">
+        <f t="shared" si="1"/>
+        <v>18.990000000000002</v>
+      </c>
+      <c r="L7" s="33"/>
+      <c r="M7" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="36">
+        <v>10</v>
+      </c>
+      <c r="O7" s="36">
+        <v>10</v>
+      </c>
+      <c r="P7" s="36">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="36">
+        <v>0</v>
+      </c>
+      <c r="R7" s="36">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="S7" s="40">
+        <v>1.899</v>
+      </c>
+      <c r="T7" s="36">
+        <f t="shared" si="3"/>
+        <v>18.990000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="11">
-        <v>60</v>
-      </c>
-      <c r="D8" s="11">
-        <v>40</v>
-      </c>
-      <c r="E8" s="11">
+      <c r="B8" s="34"/>
+      <c r="C8" s="17">
+        <f>SUM(C2:C7)</f>
+        <v>90</v>
+      </c>
+      <c r="D8" s="17">
+        <f>SUM(D2:D7)</f>
+        <v>70</v>
+      </c>
+      <c r="E8" s="17">
+        <f>SUM(E2:E7)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="17">
+        <f>SUM(F2:F7)</f>
         <v>4</v>
       </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="42">
+        <f>SUM(I2:I7) + J1</f>
+        <v>392.09414866666668</v>
+      </c>
+      <c r="L8" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="M8" s="34"/>
+      <c r="N8" s="17">
+        <f>SUM(N2:N7)</f>
+        <v>90</v>
+      </c>
+      <c r="O8" s="17">
+        <f>SUM(O2:O7)</f>
+        <v>90</v>
+      </c>
+      <c r="P8" s="17">
+        <f>SUM(P2:P7)</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="17">
+        <f>SUM(Q2:Q7)</f>
+        <v>0</v>
+      </c>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="42">
+        <f>SUM(T2:T7) + U1</f>
+        <v>499.91308200000003</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:B8"/>
+    <mergeCell ref="L2:L7"/>
+    <mergeCell ref="L8:M8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddHeader>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</oddFooter>
+    <evenHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenHeader>
+    <evenFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</evenFooter>
+    <firstHeader>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstHeader>
+    <firstFooter>&amp;L&amp;"Arial,Regular"&amp;09&amp;B&amp;U&amp;K000000TASNİF DIŞI&amp;K0000FF &amp;B&amp;K663987/ &amp;I&amp;K663987UNCLASSIFIED</firstFooter>
+  </headerFooter>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<sisl xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="753fb180-a0f1-47ee-bb6b-5956a4b631ac" origin="userSelected">
+  <element uid="id_classification_nonbusiness" value=""/>
+</sisl>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1E9475D-417F-404D-82F3-D19BBCFBE920}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
14.08.2024 tarihli okul deneme sinavi
</commit_message>
<xml_diff>
--- a/Çınar.xlsx
+++ b/Çınar.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC30F3EC-EF80-4E5E-8C01-40B315DBD8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A00547-C063-49B3-8FB5-571E50E9E109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Haftalık Plan" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="71">
   <si>
     <t>Saat</t>
   </si>
@@ -259,7 +259,7 @@
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +327,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -490,7 +498,7 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -536,74 +544,86 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="8" borderId="6" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1020,10 +1040,10 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="27" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1036,8 +1056,8 @@
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1048,10 +1068,10 @@
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="28" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1064,8 +1084,8 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1076,10 +1096,10 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="H10" s="27" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1092,8 +1112,8 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="27"/>
     </row>
     <row r="12" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1104,10 +1124,10 @@
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="H12" s="30"/>
+      <c r="H12" s="27"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -1118,8 +1138,8 @@
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="23" t="s">
+      <c r="G13" s="35"/>
+      <c r="H13" s="30" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1132,8 +1152,8 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="31"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1144,8 +1164,8 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="22" t="s">
+      <c r="G15" s="35"/>
+      <c r="H15" s="28" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1158,8 +1178,8 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="22"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="28"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
@@ -1180,8 +1200,8 @@
       <c r="F17" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="30" t="s">
+      <c r="G17" s="35"/>
+      <c r="H17" s="27" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1189,34 +1209,34 @@
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="30"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="25"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="6" t="s">
         <v>15</v>
       </c>
@@ -1225,21 +1245,21 @@
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="30" t="s">
+      <c r="C20" s="27" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="30" t="s">
+      <c r="E20" s="28"/>
+      <c r="F20" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="30" t="s">
+      <c r="G20" s="35"/>
+      <c r="H20" s="27" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1247,39 +1267,39 @@
       <c r="A21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="23" t="s">
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="30" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="30"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="24" t="s">
+      <c r="D22" s="30"/>
+      <c r="E22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="30" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1287,35 +1307,35 @@
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="27" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
     </row>
     <row r="24" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="30" t="s">
+      <c r="D24" s="33"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="H24" s="27" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1323,15 +1343,15 @@
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="22" t="s">
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="27"/>
     </row>
     <row r="26" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
@@ -1343,23 +1363,23 @@
       <c r="C26" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="27" t="s">
         <v>62</v>
       </c>
       <c r="E27" s="6" t="s">
@@ -1379,9 +1399,9 @@
       <c r="A28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
       <c r="E28" s="10" t="s">
         <v>62</v>
       </c>
@@ -1431,17 +1451,18 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G27:G30"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="G12:G21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E22:E26"/>
+    <mergeCell ref="D25:D26"/>
     <mergeCell ref="F27:F30"/>
     <mergeCell ref="H13:H14"/>
     <mergeCell ref="B20:B21"/>
@@ -1458,18 +1479,17 @@
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="D21:D22"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E22:E26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="G12:G21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G8:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -1530,7 +1550,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="37">
         <v>45549</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -1541,10 +1561,10 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="35"/>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
@@ -1553,10 +1573,10 @@
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="35"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="15" t="s">
         <v>55</v>
       </c>
@@ -1565,10 +1585,10 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="35"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="15" t="s">
         <v>56</v>
       </c>
@@ -1577,10 +1597,10 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
-      <c r="H5" s="35"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="15" t="s">
         <v>57</v>
       </c>
@@ -1589,10 +1609,10 @@
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
-      <c r="H6" s="35"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="15" t="s">
         <v>58</v>
       </c>
@@ -1601,22 +1621,22 @@
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
-      <c r="H7" s="35"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="A9" s="37">
         <v>45550</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -1627,10 +1647,10 @@
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
-      <c r="H9" s="35"/>
+      <c r="H9" s="36"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="15" t="s">
         <v>54</v>
       </c>
@@ -1639,10 +1659,10 @@
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="35"/>
+      <c r="H10" s="36"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="15" t="s">
         <v>55</v>
       </c>
@@ -1651,10 +1671,10 @@
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
-      <c r="H11" s="35"/>
+      <c r="H11" s="36"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="15" t="s">
         <v>56</v>
       </c>
@@ -1663,10 +1683,10 @@
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
-      <c r="H12" s="35"/>
+      <c r="H12" s="36"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="15" t="s">
         <v>57</v>
       </c>
@@ -1675,10 +1695,10 @@
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="35"/>
+      <c r="H13" s="36"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="33"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="15" t="s">
         <v>58</v>
       </c>
@@ -1687,22 +1707,22 @@
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="35"/>
+      <c r="H14" s="36"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="19"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="A16" s="37">
         <v>45551</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -1713,10 +1733,10 @@
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
-      <c r="H16" s="35"/>
+      <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="33"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="15" t="s">
         <v>54</v>
       </c>
@@ -1725,10 +1745,10 @@
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
-      <c r="H17" s="35"/>
+      <c r="H17" s="36"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="15" t="s">
         <v>55</v>
       </c>
@@ -1737,10 +1757,10 @@
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
-      <c r="H18" s="35"/>
+      <c r="H18" s="36"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="33"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="15" t="s">
         <v>56</v>
       </c>
@@ -1749,10 +1769,10 @@
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
-      <c r="H19" s="35"/>
+      <c r="H19" s="36"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="33"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="15" t="s">
         <v>57</v>
       </c>
@@ -1761,10 +1781,10 @@
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
-      <c r="H20" s="35"/>
+      <c r="H20" s="36"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="33"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="15" t="s">
         <v>58</v>
       </c>
@@ -1773,22 +1793,22 @@
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
-      <c r="H21" s="35"/>
+      <c r="H21" s="36"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="32">
+      <c r="A23" s="37">
         <v>45552</v>
       </c>
       <c r="B23" s="15" t="s">
@@ -1799,10 +1819,10 @@
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
-      <c r="H23" s="35"/>
+      <c r="H23" s="36"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="33"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="15" t="s">
         <v>54</v>
       </c>
@@ -1811,10 +1831,10 @@
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="36"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="33"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="15" t="s">
         <v>55</v>
       </c>
@@ -1823,10 +1843,10 @@
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
-      <c r="H25" s="35"/>
+      <c r="H25" s="36"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="15" t="s">
         <v>56</v>
       </c>
@@ -1835,10 +1855,10 @@
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
-      <c r="H26" s="35"/>
+      <c r="H26" s="36"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="15" t="s">
         <v>57</v>
       </c>
@@ -1847,10 +1867,10 @@
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
-      <c r="H27" s="35"/>
+      <c r="H27" s="36"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="15" t="s">
         <v>58</v>
       </c>
@@ -1859,22 +1879,22 @@
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
-      <c r="H28" s="35"/>
+      <c r="H28" s="36"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="19"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="32">
+      <c r="A30" s="37">
         <v>45553</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -1885,10 +1905,10 @@
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
-      <c r="H30" s="35"/>
+      <c r="H30" s="36"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="15" t="s">
         <v>54</v>
       </c>
@@ -1897,10 +1917,10 @@
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
-      <c r="H31" s="35"/>
+      <c r="H31" s="36"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="15" t="s">
         <v>55</v>
       </c>
@@ -1909,10 +1929,10 @@
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
       <c r="G32" s="15"/>
-      <c r="H32" s="35"/>
+      <c r="H32" s="36"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
+      <c r="A33" s="38"/>
       <c r="B33" s="15" t="s">
         <v>56</v>
       </c>
@@ -1921,10 +1941,10 @@
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
       <c r="G33" s="15"/>
-      <c r="H33" s="35"/>
+      <c r="H33" s="36"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="33"/>
+      <c r="A34" s="38"/>
       <c r="B34" s="15" t="s">
         <v>57</v>
       </c>
@@ -1933,10 +1953,10 @@
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
       <c r="G34" s="15"/>
-      <c r="H34" s="35"/>
+      <c r="H34" s="36"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="15" t="s">
         <v>58</v>
       </c>
@@ -1945,22 +1965,22 @@
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
       <c r="G35" s="15"/>
-      <c r="H35" s="35"/>
+      <c r="H35" s="36"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="19"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="32">
+      <c r="A37" s="37">
         <v>45554</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -1971,10 +1991,10 @@
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
       <c r="G37" s="15"/>
-      <c r="H37" s="35"/>
+      <c r="H37" s="36"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
+      <c r="A38" s="38"/>
       <c r="B38" s="15" t="s">
         <v>54</v>
       </c>
@@ -1983,10 +2003,10 @@
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15"/>
-      <c r="H38" s="35"/>
+      <c r="H38" s="36"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
+      <c r="A39" s="38"/>
       <c r="B39" s="15" t="s">
         <v>55</v>
       </c>
@@ -1995,10 +2015,10 @@
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
       <c r="G39" s="15"/>
-      <c r="H39" s="35"/>
+      <c r="H39" s="36"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
+      <c r="A40" s="38"/>
       <c r="B40" s="15" t="s">
         <v>56</v>
       </c>
@@ -2007,10 +2027,10 @@
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
       <c r="G40" s="15"/>
-      <c r="H40" s="35"/>
+      <c r="H40" s="36"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
+      <c r="A41" s="38"/>
       <c r="B41" s="15" t="s">
         <v>57</v>
       </c>
@@ -2019,10 +2039,10 @@
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
       <c r="G41" s="15"/>
-      <c r="H41" s="35"/>
+      <c r="H41" s="36"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
+      <c r="A42" s="38"/>
       <c r="B42" s="15" t="s">
         <v>58</v>
       </c>
@@ -2031,22 +2051,22 @@
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
       <c r="G42" s="15"/>
-      <c r="H42" s="35"/>
+      <c r="H42" s="36"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="34"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="19"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="18"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="32">
+      <c r="A44" s="37">
         <v>45555</v>
       </c>
       <c r="B44" s="15" t="s">
@@ -2057,10 +2077,10 @@
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
       <c r="G44" s="15"/>
-      <c r="H44" s="35"/>
+      <c r="H44" s="36"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="33"/>
+      <c r="A45" s="38"/>
       <c r="B45" s="15" t="s">
         <v>54</v>
       </c>
@@ -2069,10 +2089,10 @@
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
       <c r="G45" s="15"/>
-      <c r="H45" s="35"/>
+      <c r="H45" s="36"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="33"/>
+      <c r="A46" s="38"/>
       <c r="B46" s="15" t="s">
         <v>55</v>
       </c>
@@ -2081,10 +2101,10 @@
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
       <c r="G46" s="15"/>
-      <c r="H46" s="35"/>
+      <c r="H46" s="36"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="33"/>
+      <c r="A47" s="38"/>
       <c r="B47" s="15" t="s">
         <v>56</v>
       </c>
@@ -2093,10 +2113,10 @@
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
       <c r="G47" s="15"/>
-      <c r="H47" s="35"/>
+      <c r="H47" s="36"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="33"/>
+      <c r="A48" s="38"/>
       <c r="B48" s="15" t="s">
         <v>57</v>
       </c>
@@ -2105,10 +2125,10 @@
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="G48" s="15"/>
-      <c r="H48" s="35"/>
+      <c r="H48" s="36"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="33"/>
+      <c r="A49" s="38"/>
       <c r="B49" s="15" t="s">
         <v>58</v>
       </c>
@@ -2117,39 +2137,42 @@
       <c r="E49" s="15"/>
       <c r="F49" s="15"/>
       <c r="G49" s="15"/>
-      <c r="H49" s="35"/>
+      <c r="H49" s="36"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="34" t="s">
+      <c r="A50" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B50" s="34"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="19"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="18"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
+      <c r="A51" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="31"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
-      <c r="H51" s="21"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="H16:H21"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="H30:H35"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A50:B50"/>
     <mergeCell ref="H37:H42"/>
     <mergeCell ref="H44:H49"/>
     <mergeCell ref="A23:A28"/>
@@ -2159,14 +2182,11 @@
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="H16:H21"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="H30:H35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2186,10 +2206,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2230,7 +2250,7 @@
       <c r="I1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="41">
+      <c r="J1" s="26">
         <v>194.752082</v>
       </c>
       <c r="L1" s="12" t="s">
@@ -2260,12 +2280,12 @@
       <c r="T1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="41">
+      <c r="U1" s="26">
         <v>194.752082</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="37">
         <v>45546</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -2283,49 +2303,49 @@
       <c r="F2" s="16">
         <v>4</v>
       </c>
-      <c r="G2" s="37">
+      <c r="G2" s="22">
         <f>$D2-(E2/3)</f>
         <v>8</v>
       </c>
-      <c r="H2" s="39">
+      <c r="H2" s="24">
         <v>4.2538</v>
       </c>
-      <c r="I2" s="39">
+      <c r="I2" s="24">
         <f>$G2*H2</f>
         <v>34.0304</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="37" t="s">
         <v>70</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="36">
+      <c r="N2" s="21">
         <v>20</v>
       </c>
-      <c r="O2" s="36">
+      <c r="O2" s="21">
         <v>20</v>
       </c>
-      <c r="P2" s="36">
+      <c r="P2" s="21">
         <v>0</v>
       </c>
-      <c r="Q2" s="36">
+      <c r="Q2" s="21">
         <v>0</v>
       </c>
-      <c r="R2" s="36">
+      <c r="R2" s="21">
         <f>$O2-(P2/3)</f>
         <v>20</v>
       </c>
-      <c r="S2" s="36">
+      <c r="S2" s="21">
         <v>4.2538</v>
       </c>
-      <c r="T2" s="36">
+      <c r="T2" s="21">
         <f>$R2*S2</f>
         <v>85.075999999999993</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="15" t="s">
         <v>54</v>
       </c>
@@ -2341,47 +2361,47 @@
       <c r="F3" s="16">
         <v>0</v>
       </c>
-      <c r="G3" s="37">
+      <c r="G3" s="22">
         <f t="shared" ref="G3:G7" si="0">$D3-(E3/3)</f>
         <v>12</v>
       </c>
-      <c r="H3" s="39">
+      <c r="H3" s="24">
         <v>4.3479999999999999</v>
       </c>
-      <c r="I3" s="39">
+      <c r="I3" s="24">
         <f t="shared" ref="I3:I7" si="1">$G3*H3</f>
         <v>52.176000000000002</v>
       </c>
-      <c r="L3" s="33"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="N3" s="36">
+      <c r="N3" s="21">
         <v>20</v>
       </c>
-      <c r="O3" s="36">
+      <c r="O3" s="21">
         <v>20</v>
       </c>
-      <c r="P3" s="36">
+      <c r="P3" s="21">
         <v>0</v>
       </c>
-      <c r="Q3" s="36">
+      <c r="Q3" s="21">
         <v>0</v>
       </c>
-      <c r="R3" s="36">
+      <c r="R3" s="21">
         <f t="shared" ref="R3:R7" si="2">$O3-(P3/3)</f>
         <v>20</v>
       </c>
-      <c r="S3" s="36">
+      <c r="S3" s="21">
         <v>4.3479999999999999</v>
       </c>
-      <c r="T3" s="36">
+      <c r="T3" s="21">
         <f t="shared" ref="T3:T7" si="3">$R3*S3</f>
         <v>86.96</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="15" t="s">
         <v>55</v>
       </c>
@@ -2397,273 +2417,511 @@
       <c r="F4" s="16">
         <v>0</v>
       </c>
-      <c r="G4" s="37">
+      <c r="G4" s="22">
         <f t="shared" si="0"/>
         <v>14.666666666666666</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="24">
         <v>4.1230000000000002</v>
       </c>
-      <c r="I4" s="39">
+      <c r="I4" s="24">
         <f t="shared" si="1"/>
         <v>60.470666666666666</v>
       </c>
-      <c r="L4" s="33"/>
+      <c r="L4" s="38"/>
       <c r="M4" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="36">
+      <c r="N4" s="21">
         <v>20</v>
       </c>
-      <c r="O4" s="36">
+      <c r="O4" s="21">
         <v>20</v>
       </c>
-      <c r="P4" s="36">
+      <c r="P4" s="21">
         <v>0</v>
       </c>
-      <c r="Q4" s="36">
+      <c r="Q4" s="21">
         <v>0</v>
       </c>
-      <c r="R4" s="36">
+      <c r="R4" s="21">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="S4" s="36">
+      <c r="S4" s="21">
         <v>4.1230000000000002</v>
       </c>
-      <c r="T4" s="36">
+      <c r="T4" s="21">
         <f t="shared" si="3"/>
         <v>82.460000000000008</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="21">
         <v>10</v>
       </c>
-      <c r="D5" s="36">
+      <c r="D5" s="21">
         <v>10</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="21">
         <v>0</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="21">
         <v>0</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="25">
         <v>1.66</v>
       </c>
-      <c r="I5" s="40">
+      <c r="I5" s="25">
         <f t="shared" si="1"/>
         <v>16.599999999999998</v>
       </c>
-      <c r="L5" s="33"/>
+      <c r="L5" s="38"/>
       <c r="M5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="N5" s="36">
+      <c r="N5" s="21">
         <v>10</v>
       </c>
-      <c r="O5" s="36">
+      <c r="O5" s="21">
         <v>10</v>
       </c>
-      <c r="P5" s="36">
+      <c r="P5" s="21">
         <v>0</v>
       </c>
-      <c r="Q5" s="36">
+      <c r="Q5" s="21">
         <v>0</v>
       </c>
-      <c r="R5" s="36">
+      <c r="R5" s="21">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S5" s="40">
+      <c r="S5" s="25">
         <v>1.66</v>
       </c>
-      <c r="T5" s="36">
+      <c r="T5" s="21">
         <f t="shared" si="3"/>
         <v>16.599999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="21">
         <v>10</v>
       </c>
-      <c r="D6" s="36">
+      <c r="D6" s="21">
         <v>10</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="21">
         <v>0</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="21">
         <v>0</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H6" s="40">
+      <c r="H6" s="25">
         <v>1.5075000000000001</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="25">
         <f t="shared" si="1"/>
         <v>15.075000000000001</v>
       </c>
-      <c r="L6" s="33"/>
+      <c r="L6" s="38"/>
       <c r="M6" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="36">
+      <c r="N6" s="21">
         <v>10</v>
       </c>
-      <c r="O6" s="36">
+      <c r="O6" s="21">
         <v>10</v>
       </c>
-      <c r="P6" s="36">
+      <c r="P6" s="21">
         <v>0</v>
       </c>
-      <c r="Q6" s="36">
+      <c r="Q6" s="21">
         <v>0</v>
       </c>
-      <c r="R6" s="36">
+      <c r="R6" s="21">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S6" s="40">
+      <c r="S6" s="25">
         <v>1.5075000000000001</v>
       </c>
-      <c r="T6" s="36">
+      <c r="T6" s="21">
         <f t="shared" si="3"/>
         <v>15.075000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="21">
         <v>10</v>
       </c>
-      <c r="D7" s="36">
+      <c r="D7" s="21">
         <v>10</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="21">
         <v>0</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="21">
         <v>0</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="23">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="H7" s="40">
+      <c r="H7" s="25">
         <v>1.899</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="25">
         <f t="shared" si="1"/>
         <v>18.990000000000002</v>
       </c>
-      <c r="L7" s="33"/>
+      <c r="L7" s="38"/>
       <c r="M7" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="36">
+      <c r="N7" s="21">
         <v>10</v>
       </c>
-      <c r="O7" s="36">
+      <c r="O7" s="21">
         <v>10</v>
       </c>
-      <c r="P7" s="36">
+      <c r="P7" s="21">
         <v>0</v>
       </c>
-      <c r="Q7" s="36">
+      <c r="Q7" s="21">
         <v>0</v>
       </c>
-      <c r="R7" s="36">
+      <c r="R7" s="21">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="S7" s="40">
+      <c r="S7" s="25">
         <v>1.899</v>
       </c>
-      <c r="T7" s="36">
+      <c r="T7" s="21">
         <f t="shared" si="3"/>
         <v>18.990000000000002</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="17">
+      <c r="B8" s="44"/>
+      <c r="C8" s="45">
         <f>SUM(C2:C7)</f>
         <v>90</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="45">
         <f>SUM(D2:D7)</f>
         <v>70</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="45">
         <f>SUM(E2:E7)</f>
         <v>16</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="45">
         <f>SUM(F2:F7)</f>
         <v>4</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="42">
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="46">
         <f>SUM(I2:I7) + J1</f>
         <v>392.09414866666668</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="34"/>
-      <c r="N8" s="17">
+      <c r="M8" s="44"/>
+      <c r="N8" s="45">
         <f>SUM(N2:N7)</f>
         <v>90</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="45">
         <f>SUM(O2:O7)</f>
         <v>90</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="45">
         <f>SUM(P2:P7)</f>
         <v>0</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="45">
         <f>SUM(Q2:Q7)</f>
         <v>0</v>
       </c>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="42">
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="46">
         <f>SUM(T2:T7) + U1</f>
         <v>499.91308200000003</v>
       </c>
     </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="J11" s="26">
+        <v>194.752082</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="37">
+        <v>45553</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="16">
+        <v>20</v>
+      </c>
+      <c r="D12" s="16">
+        <v>14</v>
+      </c>
+      <c r="E12" s="16">
+        <v>4</v>
+      </c>
+      <c r="F12" s="16">
+        <v>2</v>
+      </c>
+      <c r="G12" s="22">
+        <f>$D12-(E12/3)</f>
+        <v>12.666666666666666</v>
+      </c>
+      <c r="H12" s="24">
+        <v>4.2538</v>
+      </c>
+      <c r="I12" s="24">
+        <f>$G12*H12</f>
+        <v>53.881466666666661</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="16">
+        <v>20</v>
+      </c>
+      <c r="D13" s="16">
+        <v>14</v>
+      </c>
+      <c r="E13" s="16">
+        <v>6</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="22">
+        <f t="shared" ref="G13:G17" si="4">$D13-(E13/3)</f>
+        <v>12</v>
+      </c>
+      <c r="H13" s="24">
+        <v>4.3479999999999999</v>
+      </c>
+      <c r="I13" s="24">
+        <f t="shared" ref="I13:I17" si="5">$G13*H13</f>
+        <v>52.176000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="16">
+        <v>20</v>
+      </c>
+      <c r="D14" s="16">
+        <v>16</v>
+      </c>
+      <c r="E14" s="16">
+        <v>4</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="4"/>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="H14" s="24">
+        <v>4.1230000000000002</v>
+      </c>
+      <c r="I14" s="24">
+        <f t="shared" si="5"/>
+        <v>60.470666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="41">
+        <v>10</v>
+      </c>
+      <c r="D15" s="41">
+        <v>9</v>
+      </c>
+      <c r="E15" s="41">
+        <v>1</v>
+      </c>
+      <c r="F15" s="41">
+        <v>0</v>
+      </c>
+      <c r="G15" s="42">
+        <f t="shared" si="4"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="H15" s="43">
+        <v>1.66</v>
+      </c>
+      <c r="I15" s="43">
+        <f t="shared" si="5"/>
+        <v>14.386666666666665</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="41">
+        <v>10</v>
+      </c>
+      <c r="D16" s="41">
+        <v>9</v>
+      </c>
+      <c r="E16" s="41">
+        <v>1</v>
+      </c>
+      <c r="F16" s="41">
+        <v>0</v>
+      </c>
+      <c r="G16" s="42">
+        <f t="shared" si="4"/>
+        <v>8.6666666666666661</v>
+      </c>
+      <c r="H16" s="43">
+        <v>1.5075000000000001</v>
+      </c>
+      <c r="I16" s="43">
+        <f t="shared" si="5"/>
+        <v>13.065</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="41">
+        <v>10</v>
+      </c>
+      <c r="D17" s="41">
+        <v>8</v>
+      </c>
+      <c r="E17" s="41">
+        <v>2</v>
+      </c>
+      <c r="F17" s="41">
+        <v>0</v>
+      </c>
+      <c r="G17" s="42">
+        <f t="shared" si="4"/>
+        <v>7.333333333333333</v>
+      </c>
+      <c r="H17" s="43">
+        <v>1.899</v>
+      </c>
+      <c r="I17" s="43">
+        <f t="shared" si="5"/>
+        <v>13.926</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="44"/>
+      <c r="C18" s="45">
+        <f>SUM(C12:C17)</f>
+        <v>90</v>
+      </c>
+      <c r="D18" s="45">
+        <f>SUM(D12:D17)</f>
+        <v>70</v>
+      </c>
+      <c r="E18" s="45">
+        <f>SUM(E12:E17)</f>
+        <v>18</v>
+      </c>
+      <c r="F18" s="45">
+        <f>SUM(F12:F17)</f>
+        <v>2</v>
+      </c>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="46">
+        <f>SUM(I12:I17) + J11</f>
+        <v>402.65788199999997</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="L2:L7"/>
     <mergeCell ref="L8:M8"/>
+    <mergeCell ref="A12:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>